<commit_message>
Final update of code
</commit_message>
<xml_diff>
--- a/cypress/fixtures/test-data.xlsx
+++ b/cypress/fixtures/test-data.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="14400" windowHeight="12180"/>
   </bookViews>
   <sheets>
-    <sheet name="void-refund-reasons" sheetId="1" r:id="rId1"/>
+    <sheet name="Card-types" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,15 +27,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>voidReasons</t>
+    <t>Descriptions</t>
   </si>
   <si>
-    <t>wrong punch</t>
+    <t>Credit Card</t>
   </si>
   <si>
-    <t>Incorrect Order Entry</t>
+    <t>Debit Card</t>
+  </si>
+  <si>
+    <t>Gift Card</t>
+  </si>
+  <si>
+    <t>Prepaid Card</t>
+  </si>
+  <si>
+    <t>Store Card</t>
+  </si>
+  <si>
+    <t>Master Card</t>
+  </si>
+  <si>
+    <t>Visa Card</t>
   </si>
 </sst>
 </file>
@@ -656,14 +671,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,31 +1220,79 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.8888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="21.8857142857143" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="16384" width="21.8888888888889" customWidth="1"/>
+    <col min="1" max="16384" width="21.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28.8" spans="1:1">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>